<commit_message>
update xls file for assignment 8
</commit_message>
<xml_diff>
--- a/unit8-linear optimization/FilatoiRiuniti.xlsx
+++ b/unit8-linear optimization/FilatoiRiuniti.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="2240" windowWidth="18480" windowHeight="15480" tabRatio="500"/>
+    <workbookView xWindow="15" yWindow="2235" windowWidth="18480" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="30">
   <si>
     <t>FILATOI RIUNITI - OPTIMIZING THE PRODUCTION SCHEDULE</t>
   </si>
@@ -84,21 +84,52 @@
     <t>Demand</t>
   </si>
   <si>
-    <t>Decision Variables</t>
+    <t>constraints</t>
+  </si>
+  <si>
+    <t xml:space="preserve">capacity </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>demand</t>
+  </si>
+  <si>
+    <t>LHS</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>sign</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>RHS</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;=</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Decision Variables(kg/month)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>objective($/month)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="176" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -106,12 +137,37 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -322,7 +378,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -387,16 +443,16 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -417,9 +473,14 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -747,14 +808,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E59"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="13.75" customWidth="1"/>
+    <col min="2" max="2" width="19.375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="13" t="s">
@@ -772,7 +837,7 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" ht="16" thickBot="1">
+    <row r="3" spans="1:5" ht="15" thickBot="1">
       <c r="A3" s="13" t="s">
         <v>1</v>
       </c>
@@ -781,7 +846,7 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" ht="16" thickBot="1">
+    <row r="4" spans="1:5" ht="15" thickBot="1">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -896,7 +961,7 @@
         <v>0.42499999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="16" thickBot="1">
+    <row r="11" spans="1:5" ht="15" thickBot="1">
       <c r="A11" s="9" t="s">
         <v>13</v>
       </c>
@@ -920,7 +985,7 @@
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5" ht="16" thickBot="1">
+    <row r="13" spans="1:5" ht="15" thickBot="1">
       <c r="A13" s="13" t="s">
         <v>14</v>
       </c>
@@ -929,7 +994,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" ht="16" thickBot="1">
+    <row r="14" spans="1:5" ht="15" thickBot="1">
       <c r="A14" s="2" t="s">
         <v>2</v>
       </c>
@@ -1006,7 +1071,7 @@
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:5" ht="16" thickBot="1">
+    <row r="21" spans="1:5" ht="15" thickBot="1">
       <c r="A21" s="9" t="s">
         <v>13</v>
       </c>
@@ -1024,7 +1089,7 @@
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="1:5" ht="16" thickBot="1">
+    <row r="23" spans="1:5" ht="15" thickBot="1">
       <c r="A23" s="13" t="s">
         <v>16</v>
       </c>
@@ -1033,7 +1098,7 @@
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="1:5" ht="16" thickBot="1">
+    <row r="24" spans="1:5" ht="15" thickBot="1">
       <c r="A24" s="2" t="s">
         <v>2</v>
       </c>
@@ -1148,7 +1213,7 @@
         <v>8.9</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="16" thickBot="1">
+    <row r="31" spans="1:5" ht="15" thickBot="1">
       <c r="A31" s="9" t="s">
         <v>13</v>
       </c>
@@ -1172,7 +1237,7 @@
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
     </row>
-    <row r="33" spans="1:5" ht="16" thickBot="1">
+    <row r="33" spans="1:5" ht="15" thickBot="1">
       <c r="A33" s="13" t="s">
         <v>17</v>
       </c>
@@ -1181,7 +1246,7 @@
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
     </row>
-    <row r="34" spans="1:5" ht="16" thickBot="1">
+    <row r="34" spans="1:5" ht="15" thickBot="1">
       <c r="A34" s="2" t="s">
         <v>2</v>
       </c>
@@ -1296,7 +1361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="16" thickBot="1">
+    <row r="41" spans="1:5" ht="15" thickBot="1">
       <c r="A41" s="9" t="s">
         <v>13</v>
       </c>
@@ -1320,7 +1385,7 @@
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
     </row>
-    <row r="43" spans="1:5" ht="16" thickBot="1">
+    <row r="43" spans="1:5" ht="15" thickBot="1">
       <c r="A43" s="13" t="s">
         <v>18</v>
       </c>
@@ -1329,7 +1394,7 @@
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
     </row>
-    <row r="44" spans="1:5" ht="16" thickBot="1">
+    <row r="44" spans="1:5" ht="15" thickBot="1">
       <c r="A44" s="2" t="s">
         <v>19</v>
       </c>
@@ -1373,7 +1438,7 @@
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
     </row>
-    <row r="48" spans="1:5" ht="16" thickBot="1">
+    <row r="48" spans="1:5" ht="15" thickBot="1">
       <c r="A48" s="9" t="s">
         <v>6</v>
       </c>
@@ -1398,16 +1463,16 @@
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
     </row>
-    <row r="51" spans="1:5" ht="16" thickBot="1">
+    <row r="51" spans="1:5" ht="15" thickBot="1">
       <c r="A51" s="13" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
     </row>
-    <row r="52" spans="1:5" ht="16" thickBot="1">
+    <row r="52" spans="1:5" ht="15" thickBot="1">
       <c r="A52" s="2" t="s">
         <v>2</v>
       </c>
@@ -1478,7 +1543,7 @@
       <c r="D58" s="26"/>
       <c r="E58" s="29"/>
     </row>
-    <row r="59" spans="1:5" ht="16" thickBot="1">
+    <row r="59" spans="1:5" ht="15" thickBot="1">
       <c r="A59" s="9" t="s">
         <v>13</v>
       </c>
@@ -1487,7 +1552,157 @@
       <c r="D59" s="30"/>
       <c r="E59" s="31"/>
     </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="C61">
+        <f>SUMPRODUCT(B53:E59,B25:E31)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="32" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="32"/>
+      <c r="C64" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="D64" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="E64" s="33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" t="s">
+        <v>22</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C65" s="34">
+        <f>SUM(B53:E53)</f>
+        <v>0</v>
+      </c>
+      <c r="D65" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="E65">
+        <f>B15</f>
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="B66" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C66" s="34">
+        <f t="shared" ref="C66:C71" si="0">SUM(B54:E54)</f>
+        <v>0</v>
+      </c>
+      <c r="D66" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="E66">
+        <f t="shared" ref="E66:E71" si="1">B16</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="B67" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C67" s="34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D67" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="E67">
+        <f t="shared" si="1"/>
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="B68" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C68" s="34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D68" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="E68">
+        <f t="shared" si="1"/>
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="B69" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C69" s="34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D69" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="E69">
+        <f t="shared" si="1"/>
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="B70" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C70" s="34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D70" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="E70">
+        <f t="shared" si="1"/>
+        <v>38000</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="15" thickBot="1">
+      <c r="B71" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C71" s="34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D71" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="E71">
+        <f t="shared" si="1"/>
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" t="s">
+        <v>23</v>
+      </c>
+      <c r="B72" s="34"/>
+      <c r="C72" s="34"/>
+      <c r="D72" s="34"/>
+    </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>